<commit_message>
Final Results to write up including Yu test with Dioguardi, Initial Velocity Assumption Test, Fluid Density Assumption Test and constant terminal velocity test. 22.07.22
</commit_message>
<xml_diff>
--- a/Output/20220517/StokesCheckProjAESDWt.xlsx
+++ b/Output/20220517/StokesCheckProjAESDWt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roisi\Desktop\mP Model Code\DragModelsTest\Output\20220517\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B87FF6F-79BD-48D4-A26C-A26BA4BCDB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E333DB-4A44-4BA3-9960-87854EF41481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A7FCB9C0-3200-4839-92C8-D5422E6FBE56}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>x1</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At terminal settling velocity when the net force </t>
   </si>
 </sst>
 </file>
@@ -4054,6 +4057,815 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AB$3:$AB$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$3:$AD$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-449B-4B25-B533-8D9BEA5C3CCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AB$13:$AB$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$13:$AD$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-449B-4B25-B533-8D9BEA5C3CCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AB$23:$AB$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$23:$AD$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-449B-4B25-B533-8D9BEA5C3CCD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1563997375"/>
+        <c:axId val="1564000703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1563997375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>ESD</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1564000703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1564000703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Wt+1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1563997375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4254,6 +5066,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6319,6 +7171,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7016,6 +8384,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>51163</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>355963</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A16D3578-8B92-7867-3637-DF6CBB908A3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7316,15 +8720,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9A395F-7D31-4337-A228-E26D34F466B4}">
-  <dimension ref="B1:R43"/>
+  <dimension ref="B1:AF43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -7343,8 +8747,14 @@
       <c r="R1" t="s">
         <v>5</v>
       </c>
+      <c r="AB1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -7369,8 +8779,17 @@
       <c r="R2" t="s">
         <v>6</v>
       </c>
+      <c r="AB2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -7394,11 +8813,21 @@
         <v>5</v>
       </c>
       <c r="R3">
-        <f>(Q3*P3*P3*O3)+O3+Q3</f>
+        <f t="shared" ref="R3:R32" si="0">(Q3*P3*P3*O3)+O3+Q3</f>
         <v>26</v>
       </c>
+      <c r="AB3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>5</v>
+      </c>
+      <c r="AD3">
+        <f>AC3*AB3*AB3</f>
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -7409,7 +8838,7 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E32" si="0">(D4*C4*C4*B4)+B4+D4</f>
+        <f t="shared" ref="E4:E32" si="1">(D4*C4*C4*B4)+B4+D4</f>
         <v>47</v>
       </c>
       <c r="O4">
@@ -7422,11 +8851,21 @@
         <v>5</v>
       </c>
       <c r="R4">
-        <f>(Q4*P4*P4*O4)+O4+Q4</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+      <c r="AC4">
+        <v>5</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD32" si="2">AC4*AB4*AB4</f>
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -7437,752 +8876,1025 @@
         <v>5</v>
       </c>
       <c r="E5">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="AB5">
+        <v>4</v>
+      </c>
+      <c r="AC5">
+        <v>5</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="AB6">
+        <v>5</v>
+      </c>
+      <c r="AC6">
+        <v>5</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+      <c r="AB7">
+        <v>6</v>
+      </c>
+      <c r="AC7">
+        <v>5</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+      <c r="AB8">
+        <v>7</v>
+      </c>
+      <c r="AC8">
+        <v>5</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="2"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>8</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+      <c r="AB9">
+        <v>8</v>
+      </c>
+      <c r="AC9">
+        <v>5</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>9</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+      <c r="AB10">
+        <v>9</v>
+      </c>
+      <c r="AC10">
+        <v>5</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="2"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>248</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
+      <c r="AB11">
+        <v>10</v>
+      </c>
+      <c r="AC11">
+        <v>5</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>611</v>
+      </c>
+      <c r="AB12">
+        <v>11</v>
+      </c>
+      <c r="AC12">
+        <v>5</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="2"/>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>257</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
+      </c>
+      <c r="AC13">
+        <v>10</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>383</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>5</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="AB14">
+        <v>3</v>
+      </c>
+      <c r="AC14">
+        <v>10</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>186</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>4</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="AB15">
+        <v>4</v>
+      </c>
+      <c r="AC15">
+        <v>10</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>367</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>257</v>
+      </c>
+      <c r="AB16">
+        <v>5</v>
+      </c>
+      <c r="AC16">
+        <v>10</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>548</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>367</v>
+      </c>
+      <c r="AB17">
+        <v>6</v>
+      </c>
+      <c r="AC17">
+        <v>10</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>7</v>
+      </c>
+      <c r="Q18">
+        <v>5</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+      <c r="AB18">
+        <v>7</v>
+      </c>
+      <c r="AC18">
+        <v>10</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="2"/>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>497</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+      <c r="AB19">
+        <v>8</v>
+      </c>
+      <c r="AC19">
+        <v>10</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="2"/>
+        <v>640</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>743</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>9</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="0"/>
+        <v>817</v>
+      </c>
+      <c r="AB20">
+        <v>9</v>
+      </c>
+      <c r="AC20">
+        <v>10</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="2"/>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>326</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>10</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="0"/>
+        <v>1007</v>
+      </c>
+      <c r="AB21">
+        <v>10</v>
+      </c>
+      <c r="AC21">
+        <v>10</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>647</v>
+      </c>
+      <c r="O22">
+        <v>2</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>1217</v>
+      </c>
+      <c r="AB22">
+        <v>11</v>
+      </c>
+      <c r="AC22">
+        <v>10</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="2"/>
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>968</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="O5">
+      <c r="AB23">
+        <v>2</v>
+      </c>
+      <c r="AC23">
+        <v>15</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="P5">
-        <v>4</v>
-      </c>
-      <c r="Q5">
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
         <v>5</v>
       </c>
-      <c r="R5">
-        <f>(Q5*P5*P5*O5)+O5+Q5</f>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="O24">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
         <v>5</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>5</v>
-      </c>
-      <c r="Q6">
-        <v>5</v>
-      </c>
-      <c r="R6">
-        <f>(Q6*P6*P6*O6)+O6+Q6</f>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>6</v>
-      </c>
-      <c r="Q7">
-        <v>5</v>
-      </c>
-      <c r="R7">
-        <f>(Q7*P7*P7*O7)+O7+Q7</f>
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
+      <c r="R24">
         <f t="shared" si="0"/>
         <v>143</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>7</v>
-      </c>
-      <c r="Q8">
+      <c r="AB24">
+        <v>3</v>
+      </c>
+      <c r="AC24">
+        <v>15</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+      <c r="D25">
         <v>5</v>
       </c>
-      <c r="R8">
-        <f>(Q8*P8*P8*O8)+O8+Q8</f>
-        <v>251</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>817</v>
+      </c>
+      <c r="O25">
+        <v>3</v>
+      </c>
+      <c r="P25">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="Q25">
         <v>5</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>8</v>
-      </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="R9">
-        <f>(Q9*P9*P9*O9)+O9+Q9</f>
-        <v>326</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>167</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>9</v>
-      </c>
-      <c r="Q10">
-        <v>5</v>
-      </c>
-      <c r="R10">
-        <f>(Q10*P10*P10*O10)+O10+Q10</f>
-        <v>411</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="E11">
+      <c r="R25">
         <f t="shared" si="0"/>
         <v>248</v>
       </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>10</v>
-      </c>
-      <c r="Q11">
+      <c r="AB25">
+        <v>4</v>
+      </c>
+      <c r="AC25">
+        <v>15</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="R11">
-        <f>(Q11*P11*P11*O11)+O11+Q11</f>
-        <v>506</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1223</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
+      </c>
+      <c r="P26">
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="Q26">
         <v>5</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>131</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>11</v>
-      </c>
-      <c r="Q12">
-        <v>5</v>
-      </c>
-      <c r="R12">
-        <f>(Q12*P12*P12*O12)+O12+Q12</f>
-        <v>611</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>257</v>
-      </c>
-      <c r="O13">
-        <v>2</v>
-      </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
-      <c r="Q13">
-        <v>5</v>
-      </c>
-      <c r="R13">
-        <f>(Q13*P13*P13*O13)+O13+Q13</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
+      <c r="R26">
         <f t="shared" si="0"/>
         <v>383</v>
       </c>
-      <c r="O14">
-        <v>2</v>
-      </c>
-      <c r="P14">
+      <c r="AB26">
+        <v>5</v>
+      </c>
+      <c r="AC26">
+        <v>15</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>506</v>
+      </c>
+      <c r="O27">
         <v>3</v>
       </c>
-      <c r="Q14">
+      <c r="P27">
+        <v>6</v>
+      </c>
+      <c r="Q27">
         <v>5</v>
       </c>
-      <c r="R14">
-        <f>(Q14*P14*P14*O14)+O14+Q14</f>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-      <c r="O15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <v>4</v>
-      </c>
-      <c r="Q15">
-        <v>5</v>
-      </c>
-      <c r="R15">
-        <f>(Q15*P15*P15*O15)+O15+Q15</f>
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>367</v>
-      </c>
-      <c r="O16">
-        <v>2</v>
-      </c>
-      <c r="P16">
-        <v>5</v>
-      </c>
-      <c r="Q16">
-        <v>5</v>
-      </c>
-      <c r="R16">
-        <f>(Q16*P16*P16*O16)+O16+Q16</f>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17">
+      <c r="R27">
         <f t="shared" si="0"/>
         <v>548</v>
       </c>
-      <c r="O17">
+      <c r="AB27">
+        <v>6</v>
+      </c>
+      <c r="AC27">
+        <v>15</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="2"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>2</v>
       </c>
-      <c r="P17">
-        <v>6</v>
-      </c>
-      <c r="Q17">
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
         <v>5</v>
       </c>
-      <c r="R17">
-        <f>(Q17*P17*P17*O17)+O17+Q17</f>
-        <v>367</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>1007</v>
+      </c>
+      <c r="O28">
+        <v>3</v>
+      </c>
+      <c r="P28">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="Q28">
         <v>5</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>251</v>
-      </c>
-      <c r="O18">
-        <v>2</v>
-      </c>
-      <c r="P18">
-        <v>7</v>
-      </c>
-      <c r="Q18">
-        <v>5</v>
-      </c>
-      <c r="R18">
-        <f>(Q18*P18*P18*O18)+O18+Q18</f>
-        <v>497</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-      <c r="O19">
-        <v>2</v>
-      </c>
-      <c r="P19">
-        <v>8</v>
-      </c>
-      <c r="Q19">
-        <v>5</v>
-      </c>
-      <c r="R19">
-        <f>(Q19*P19*P19*O19)+O19+Q19</f>
-        <v>647</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>7</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20">
+      <c r="R28">
         <f t="shared" si="0"/>
         <v>743</v>
       </c>
-      <c r="O20">
-        <v>2</v>
-      </c>
-      <c r="P20">
-        <v>9</v>
-      </c>
-      <c r="Q20">
+      <c r="AB28">
+        <v>7</v>
+      </c>
+      <c r="AC28">
+        <v>15</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="2"/>
+        <v>735</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
         <v>5</v>
       </c>
-      <c r="R20">
-        <f>(Q20*P20*P20*O20)+O20+Q20</f>
-        <v>817</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1508</v>
+      </c>
+      <c r="O29">
+        <v>3</v>
+      </c>
+      <c r="P29">
         <v>8</v>
       </c>
-      <c r="D21">
+      <c r="Q29">
         <v>5</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>326</v>
-      </c>
-      <c r="O21">
-        <v>2</v>
-      </c>
-      <c r="P21">
-        <v>10</v>
-      </c>
-      <c r="Q21">
-        <v>5</v>
-      </c>
-      <c r="R21">
-        <f>(Q21*P21*P21*O21)+O21+Q21</f>
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>8</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>647</v>
-      </c>
-      <c r="O22">
-        <v>2</v>
-      </c>
-      <c r="P22">
-        <v>11</v>
-      </c>
-      <c r="Q22">
-        <v>5</v>
-      </c>
-      <c r="R22">
-        <f>(Q22*P22*P22*O22)+O22+Q22</f>
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-      <c r="E23">
+      <c r="R29">
         <f t="shared" si="0"/>
         <v>968</v>
       </c>
-      <c r="O23">
+      <c r="AB29">
+        <v>8</v>
+      </c>
+      <c r="AC29">
+        <v>15</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="2"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>611</v>
+      </c>
+      <c r="O30">
         <v>3</v>
       </c>
-      <c r="P23">
-        <v>2</v>
-      </c>
-      <c r="Q23">
+      <c r="P30">
+        <v>9</v>
+      </c>
+      <c r="Q30">
         <v>5</v>
       </c>
-      <c r="R23">
-        <f>(Q23*P23*P23*O23)+O23+Q23</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>411</v>
-      </c>
-      <c r="O24">
-        <v>3</v>
-      </c>
-      <c r="P24">
-        <v>3</v>
-      </c>
-      <c r="Q24">
-        <v>5</v>
-      </c>
-      <c r="R24">
-        <f>(Q24*P24*P24*O24)+O24+Q24</f>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25">
-        <v>5</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>817</v>
-      </c>
-      <c r="O25">
-        <v>3</v>
-      </c>
-      <c r="P25">
-        <v>4</v>
-      </c>
-      <c r="Q25">
-        <v>5</v>
-      </c>
-      <c r="R25">
-        <f>(Q25*P25*P25*O25)+O25+Q25</f>
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>9</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
-      </c>
-      <c r="E26">
+      <c r="R30">
         <f t="shared" si="0"/>
         <v>1223</v>
       </c>
-      <c r="O26">
+      <c r="AB30">
+        <v>9</v>
+      </c>
+      <c r="AC30">
+        <v>15</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="2"/>
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1217</v>
+      </c>
+      <c r="O31">
         <v>3</v>
       </c>
-      <c r="P26">
+      <c r="P31">
+        <v>10</v>
+      </c>
+      <c r="Q31">
         <v>5</v>
       </c>
-      <c r="Q26">
-        <v>5</v>
-      </c>
-      <c r="R26">
-        <f>(Q26*P26*P26*O26)+O26+Q26</f>
-        <v>383</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>506</v>
-      </c>
-      <c r="O27">
-        <v>3</v>
-      </c>
-      <c r="P27">
-        <v>6</v>
-      </c>
-      <c r="Q27">
-        <v>5</v>
-      </c>
-      <c r="R27">
-        <f>(Q27*P27*P27*O27)+O27+Q27</f>
-        <v>548</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>10</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>1007</v>
-      </c>
-      <c r="O28">
-        <v>3</v>
-      </c>
-      <c r="P28">
-        <v>7</v>
-      </c>
-      <c r="Q28">
-        <v>5</v>
-      </c>
-      <c r="R28">
-        <f>(Q28*P28*P28*O28)+O28+Q28</f>
-        <v>743</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>10</v>
-      </c>
-      <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29">
+      <c r="R31">
         <f t="shared" si="0"/>
         <v>1508</v>
       </c>
-      <c r="O29">
-        <v>3</v>
-      </c>
-      <c r="P29">
-        <v>8</v>
-      </c>
-      <c r="Q29">
-        <v>5</v>
-      </c>
-      <c r="R29">
-        <f>(Q29*P29*P29*O29)+O29+Q29</f>
-        <v>968</v>
+      <c r="AB31">
+        <v>10</v>
+      </c>
+      <c r="AC31">
+        <v>15</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="2"/>
+        <v>1500</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>611</v>
-      </c>
-      <c r="O30">
-        <v>3</v>
-      </c>
-      <c r="P30">
-        <v>9</v>
-      </c>
-      <c r="Q30">
-        <v>5</v>
-      </c>
-      <c r="R30">
-        <f>(Q30*P30*P30*O30)+O30+Q30</f>
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>11</v>
-      </c>
-      <c r="D31">
-        <v>5</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>1217</v>
-      </c>
-      <c r="O31">
-        <v>3</v>
-      </c>
-      <c r="P31">
-        <v>10</v>
-      </c>
-      <c r="Q31">
-        <v>5</v>
-      </c>
-      <c r="R31">
-        <f>(Q31*P31*P31*O31)+O31+Q31</f>
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>3</v>
       </c>
@@ -8193,21 +9905,31 @@
         <v>5</v>
       </c>
       <c r="E32">
+        <f t="shared" si="1"/>
+        <v>1823</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="P32">
+        <v>11</v>
+      </c>
+      <c r="Q32">
+        <v>5</v>
+      </c>
+      <c r="R32">
         <f t="shared" si="0"/>
         <v>1823</v>
       </c>
-      <c r="O32">
-        <v>3</v>
-      </c>
-      <c r="P32">
+      <c r="AB32">
         <v>11</v>
       </c>
-      <c r="Q32">
-        <v>5</v>
-      </c>
-      <c r="R32">
-        <f>(Q32*P32*P32*O32)+O32+Q32</f>
-        <v>1823</v>
+      <c r="AC32">
+        <v>15</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="2"/>
+        <v>1815</v>
       </c>
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.3">

</xml_diff>